<commit_message>
Ajout du choix du fichier eba et carte de visualisation des chocs
</commit_message>
<xml_diff>
--- a/output/analyse_poste.xlsx
+++ b/output/analyse_poste.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BO2"/>
+  <dimension ref="A1:BO3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,202 +777,407 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27022068187.41332</v>
+        <v>13511034093.70666</v>
       </c>
       <c r="C2" t="n">
-        <v>26872214412.7774</v>
+        <v>13436107206.3887</v>
       </c>
       <c r="D2" t="n">
-        <v>26770838612.00669</v>
+        <v>13385419306.00335</v>
       </c>
       <c r="E2" t="n">
-        <v>24633369746.45487</v>
+        <v>12316684873.22743</v>
       </c>
       <c r="F2" t="n">
-        <v>22861742959.95803</v>
+        <v>11430871479.97902</v>
       </c>
       <c r="G2" t="n">
-        <v>22770462461.7534</v>
+        <v>11385231230.8767</v>
       </c>
       <c r="H2" t="n">
-        <v>22676588359.01294</v>
+        <v>11338294179.50647</v>
       </c>
       <c r="I2" t="n">
-        <v>22585689924.29336</v>
+        <v>11292844962.14668</v>
       </c>
       <c r="J2" t="n">
-        <v>22492209563.53871</v>
+        <v>11246104781.76936</v>
       </c>
       <c r="K2" t="n">
-        <v>22608791015.02794</v>
+        <v>11304395507.51397</v>
       </c>
       <c r="L2" t="n">
-        <v>22532014830.50699</v>
+        <v>11266007415.25349</v>
       </c>
       <c r="M2" t="n">
-        <v>22458952031.13441</v>
+        <v>11229476015.5672</v>
       </c>
       <c r="N2" t="n">
-        <v>22390412205.69703</v>
+        <v>11195206102.84851</v>
       </c>
       <c r="O2" t="n">
-        <v>22319880102.44408</v>
+        <v>11159940051.22204</v>
       </c>
       <c r="P2" t="n">
-        <v>22251540074.75029</v>
+        <v>11125770037.37515</v>
       </c>
       <c r="Q2" t="n">
-        <v>22181213876.43439</v>
+        <v>11090606938.2172</v>
       </c>
       <c r="R2" t="n">
-        <v>22112032902.08925</v>
+        <v>11056016451.04463</v>
       </c>
       <c r="S2" t="n">
-        <v>22043992571.17704</v>
+        <v>11021996285.58852</v>
       </c>
       <c r="T2" t="n">
-        <v>21973975230.56987</v>
+        <v>10986987615.28494</v>
       </c>
       <c r="U2" t="n">
-        <v>21906134697.34366</v>
+        <v>10953067348.67183</v>
       </c>
       <c r="V2" t="n">
-        <v>21836323262.0247</v>
+        <v>10918161631.01235</v>
       </c>
       <c r="W2" t="n">
-        <v>22008140934.56245</v>
+        <v>11004070467.28123</v>
       </c>
       <c r="X2" t="n">
-        <v>21948195255.88668</v>
+        <v>10974097627.94334</v>
       </c>
       <c r="Y2" t="n">
-        <v>21883155341.63987</v>
+        <v>10941577670.81993</v>
       </c>
       <c r="Z2" t="n">
-        <v>21822126140.59001</v>
+        <v>10911063070.295</v>
       </c>
       <c r="AA2" t="n">
-        <v>21759307184.47539</v>
+        <v>10879653592.23769</v>
       </c>
       <c r="AB2" t="n">
-        <v>21698425203.02333</v>
+        <v>10849212601.51167</v>
       </c>
       <c r="AC2" t="n">
-        <v>21635757967.04953</v>
+        <v>10817878983.52477</v>
       </c>
       <c r="AD2" t="n">
-        <v>21574095460.58501</v>
+        <v>10787047730.29251</v>
       </c>
       <c r="AE2" t="n">
-        <v>21513434308.13003</v>
+        <v>10756717154.06502</v>
       </c>
       <c r="AF2" t="n">
-        <v>21450994650.96572</v>
+        <v>10725497325.48286</v>
       </c>
       <c r="AG2" t="n">
-        <v>21390480718.22331</v>
+        <v>10695240359.11165</v>
       </c>
       <c r="AH2" t="n">
-        <v>21328192781.0108</v>
+        <v>10664096390.5054</v>
       </c>
       <c r="AI2" t="n">
-        <v>21550628014.63436</v>
+        <v>10775314007.31718</v>
       </c>
       <c r="AJ2" t="n">
-        <v>21488761233.22154</v>
+        <v>10744380616.61077</v>
       </c>
       <c r="AK2" t="n">
-        <v>21421861819.8537</v>
+        <v>10710930909.92685</v>
       </c>
       <c r="AL2" t="n">
-        <v>21359094567.9148</v>
+        <v>10679547283.9574</v>
       </c>
       <c r="AM2" t="n">
-        <v>21294493452.32474</v>
+        <v>10647246726.16237</v>
       </c>
       <c r="AN2" t="n">
-        <v>21231890945.50145</v>
+        <v>10615945472.75072</v>
       </c>
       <c r="AO2" t="n">
-        <v>21167459611.33434</v>
+        <v>10583729805.66717</v>
       </c>
       <c r="AP2" t="n">
-        <v>21104068138.75372</v>
+        <v>10552034069.37686</v>
       </c>
       <c r="AQ2" t="n">
-        <v>21041712750.57485</v>
+        <v>10520856375.28743</v>
       </c>
       <c r="AR2" t="n">
-        <v>20977536088.52466</v>
+        <v>10488768044.26233</v>
       </c>
       <c r="AS2" t="n">
-        <v>20915345445.78153</v>
+        <v>10457672722.89077</v>
       </c>
       <c r="AT2" t="n">
-        <v>20851338565.10534</v>
+        <v>10425669282.55267</v>
       </c>
       <c r="AU2" t="n">
-        <v>21118875073.98354</v>
+        <v>10559437536.99177</v>
       </c>
       <c r="AV2" t="n">
-        <v>21054039270.39461</v>
+        <v>10527019635.1973</v>
       </c>
       <c r="AW2" t="n">
-        <v>20986483265.79972</v>
+        <v>10493241632.89986</v>
       </c>
       <c r="AX2" t="n">
-        <v>20922046058.54723</v>
+        <v>10461023029.27361</v>
       </c>
       <c r="AY2" t="n">
-        <v>20855732961.37386</v>
+        <v>10427866480.68693</v>
       </c>
       <c r="AZ2" t="n">
-        <v>20791478025.92056</v>
+        <v>10395739012.96028</v>
       </c>
       <c r="BA2" t="n">
-        <v>20725352771.69978</v>
+        <v>10362676385.84989</v>
       </c>
       <c r="BB2" t="n">
-        <v>20660301469.95463</v>
+        <v>10330150734.97732</v>
       </c>
       <c r="BC2" t="n">
-        <v>20596319942.00052</v>
+        <v>10298159971.00026</v>
       </c>
       <c r="BD2" t="n">
-        <v>20530476452.73529</v>
+        <v>10265238226.36765</v>
       </c>
       <c r="BE2" t="n">
-        <v>20466677196.33392</v>
+        <v>10233338598.16696</v>
       </c>
       <c r="BF2" t="n">
-        <v>20401021550.54495</v>
+        <v>10200510775.27247</v>
       </c>
       <c r="BG2" t="n">
-        <v>20661458237.67993</v>
+        <v>10330729118.83997</v>
       </c>
       <c r="BH2" t="n">
-        <v>20598292385.7767</v>
+        <v>10299146192.88835</v>
       </c>
       <c r="BI2" t="n">
-        <v>20530195778.47669</v>
+        <v>10265097889.23834</v>
       </c>
       <c r="BJ2" t="n">
-        <v>23857078508.65651</v>
+        <v>11928539254.32825</v>
       </c>
       <c r="BK2" t="n">
-        <v>22071249704.55161</v>
+        <v>11035624852.2758</v>
       </c>
       <c r="BL2" t="n">
-        <v>21552838790.14689</v>
+        <v>10776419395.07345</v>
       </c>
       <c r="BM2" t="n">
-        <v>21091861431.33278</v>
+        <v>10545930715.66639</v>
       </c>
       <c r="BN2" t="n">
-        <v>20644946069.25367</v>
+        <v>10322473034.62684</v>
       </c>
       <c r="BO2" t="n">
-        <v>1419833668551.239</v>
+        <v>709916834275.6194</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>EBA_Adverse_2023_Euro Area</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>43437974611.26691</v>
+      </c>
+      <c r="C3" t="n">
+        <v>43089214286.76186</v>
+      </c>
+      <c r="D3" t="n">
+        <v>42819464544.53368</v>
+      </c>
+      <c r="E3" t="n">
+        <v>39302232384.96671</v>
+      </c>
+      <c r="F3" t="n">
+        <v>36384538308.79318</v>
+      </c>
+      <c r="G3" t="n">
+        <v>36148769562.17599</v>
+      </c>
+      <c r="H3" t="n">
+        <v>35909844294.94889</v>
+      </c>
+      <c r="I3" t="n">
+        <v>35676587278.28384</v>
+      </c>
+      <c r="J3" t="n">
+        <v>35440203044.94714</v>
+      </c>
+      <c r="K3" t="n">
+        <v>35534937581.16471</v>
+      </c>
+      <c r="L3" t="n">
+        <v>35325830696.86799</v>
+      </c>
+      <c r="M3" t="n">
+        <v>35123353901.93518</v>
+      </c>
+      <c r="N3" t="n">
+        <v>34928723832.51679</v>
+      </c>
+      <c r="O3" t="n">
+        <v>34731746623.20664</v>
+      </c>
+      <c r="P3" t="n">
+        <v>34538937923.35239</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>34343800348.94737</v>
+      </c>
+      <c r="R3" t="n">
+        <v>34151190732.31499</v>
+      </c>
+      <c r="S3" t="n">
+        <v>33961086191.15508</v>
+      </c>
+      <c r="T3" t="n">
+        <v>33768679949.07453</v>
+      </c>
+      <c r="U3" t="n">
+        <v>33580359744.60448</v>
+      </c>
+      <c r="V3" t="n">
+        <v>33389755806.77682</v>
+      </c>
+      <c r="W3" t="n">
+        <v>33568445001.21838</v>
+      </c>
+      <c r="X3" t="n">
+        <v>33393413691.6041</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>33211315872.4902</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>33035990996.91408</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>32858631950.89892</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>32684870400.62279</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>32509089315.11255</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>32335488221.02354</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>32164048519.80388</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>31990611061.22994</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>31820703965.39169</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>31648813516.50626</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>31899027553.33814</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>31728024395.38707</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>31550264272.50764</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>31379264770.38698</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>31206235100.19546</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>31036795489.93167</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>30865340815.27256</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>30696061390.39668</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>30528938163.37262</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>30359822344.10468</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>30194227869.0374</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>30026655663.15125</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>30335973907.93168</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>30167319778.5042</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>29995430881.90837</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>29828658821.35775</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>29659864843.1464</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>29494647565.85694</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>29327423888.9861</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>29162367361.43184</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>28999458533.48527</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>28834566394.46665</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>28673180852.92392</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>28509827267.5046</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>28801677191.81573</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>28641922454.81038</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>28475946890.25993</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>33007792496.98387</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>30460728255.69936</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>29670985810.24386</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>28963866837.49675</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>28279356492.252</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>2113570308515.559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>